<commit_message>
Config Server and Discovey  microservice created
Signed-off-by: Prashant <tanspra@gmail.com>
</commit_message>
<xml_diff>
--- a/resource/Notes.xlsx
+++ b/resource/Notes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Local_setup" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Status</t>
   </si>
@@ -82,6 +82,27 @@
   </si>
   <si>
     <t>1CTYKZ61N3</t>
+  </si>
+  <si>
+    <t>Gtaeway</t>
+  </si>
+  <si>
+    <t>Microservice</t>
+  </si>
+  <si>
+    <t>Dependency</t>
+  </si>
+  <si>
+    <t>Gateway (Spring cloud routing)</t>
+  </si>
+  <si>
+    <t>Eureka Discovery Client</t>
+  </si>
+  <si>
+    <t>Config Client</t>
+  </si>
+  <si>
+    <t>Spring boot Actuator</t>
   </si>
 </sst>
 </file>
@@ -111,7 +132,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -121,6 +142,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -152,7 +179,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -169,6 +196,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,7 +493,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -588,12 +616,50 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Business microservices Studen and School has been created
Signed-off-by: Prashant <tanspra@gmail.com>
</commit_message>
<xml_diff>
--- a/resource/Notes.xlsx
+++ b/resource/Notes.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
   <si>
     <t>Status</t>
   </si>
@@ -103,6 +103,36 @@
   </si>
   <si>
     <t>Spring boot Actuator</t>
+  </si>
+  <si>
+    <t>Student</t>
+  </si>
+  <si>
+    <t>Postgre sql</t>
+  </si>
+  <si>
+    <t>Lombok</t>
+  </si>
+  <si>
+    <t>Spring data jpa</t>
+  </si>
+  <si>
+    <t>Spring Web</t>
+  </si>
+  <si>
+    <t>config client</t>
+  </si>
+  <si>
+    <t>Eureka discovery client</t>
+  </si>
+  <si>
+    <t>Spring Boot Actuator</t>
+  </si>
+  <si>
+    <t>Port</t>
+  </si>
+  <si>
+    <t>School</t>
   </si>
 </sst>
 </file>
@@ -616,10 +646,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -628,35 +658,123 @@
     <col min="2" max="2" width="28.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="8" t="s">
         <v>22</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>21</v>
       </c>
       <c r="B2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2">
+        <v>8090</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="B3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:3">
       <c r="B4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:3">
       <c r="B5" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7">
+        <v>8091</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15">
+        <v>8092</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2">
+      <c r="B17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2">
+      <c r="B18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2">
+      <c r="B19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2">
+      <c r="B20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2">
+      <c r="B21" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Postgresql installed and configured on local system
Signed-off-by: Prashant <tanspra@gmail.com>
</commit_message>
<xml_diff>
--- a/resource/Notes.xlsx
+++ b/resource/Notes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="Local_setup" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="41">
   <si>
     <t>Status</t>
   </si>
@@ -133,6 +133,20 @@
   </si>
   <si>
     <t>School</t>
+  </si>
+  <si>
+    <t>postgresql</t>
+  </si>
+  <si>
+    <t>initialize server :
+initdb.exe -U admin -A password -W -E utf8  -D C:\PostGreSQL\data
+To start db server :
+pg_ctl -D ^"C^:^\PostGreSQL^\data^" -l logfile start</t>
+  </si>
+  <si>
+    <t>installed
+username : admin
+password : admin@123</t>
   </si>
 </sst>
 </file>
@@ -523,15 +537,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="21.42578125" customWidth="1"/>
     <col min="2" max="2" width="40" customWidth="1"/>
-    <col min="3" max="3" width="45.42578125" customWidth="1"/>
+    <col min="3" max="3" width="61.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -556,6 +570,17 @@
       </c>
       <c r="B3" s="3" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="75">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -648,7 +673,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
school to student connection in progress
Signed-off-by: Prashant <tanspra@gmail.com>
</commit_message>
<xml_diff>
--- a/resource/Notes.xlsx
+++ b/resource/Notes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Local_setup" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="43">
   <si>
     <t>Status</t>
   </si>
@@ -147,6 +147,12 @@
     <t>installed
 username : admin
 password : admin@123</t>
+  </si>
+  <si>
+    <t>pg_ctl -D ^"C^:^\PostGreSQL^\data^" -l logfile start</t>
+  </si>
+  <si>
+    <t>openfeign</t>
   </si>
 </sst>
 </file>
@@ -535,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -548,7 +554,7 @@
     <col min="3" max="3" width="61.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -556,7 +562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -564,7 +570,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -572,7 +578,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="75">
+    <row r="4" spans="1:4" ht="75">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -582,8 +588,11 @@
       <c r="C4" s="4" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -591,12 +600,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="30">
+    <row r="6" spans="1:4" ht="30">
       <c r="B6" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -604,7 +613,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -612,7 +621,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="45">
+    <row r="10" spans="1:4" ht="45">
       <c r="B10" s="5" t="s">
         <v>13</v>
       </c>
@@ -620,7 +629,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="18.75">
+    <row r="12" spans="1:4" ht="18.75">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -671,10 +680,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -802,6 +811,11 @@
         <v>35</v>
       </c>
     </row>
+    <row r="22" spans="2:2">
+      <c r="B22" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
school to student integration completed
Signed-off-by: Prashant <tanspra@gmail.com>
</commit_message>
<xml_diff>
--- a/resource/Notes.xlsx
+++ b/resource/Notes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="Local_setup" sheetId="1" r:id="rId1"/>
@@ -543,7 +543,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -682,7 +682,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>

</xml_diff>